<commit_message>
plot mods fixes #89
</commit_message>
<xml_diff>
--- a/paper/Table_1.xlsx
+++ b/paper/Table_1.xlsx
@@ -47,6 +47,18 @@
     <t xml:space="preserve">Percent_uci</t>
   </si>
   <si>
+    <t xml:space="preserve">Switzerland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.9%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.5%</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sweden</t>
   </si>
   <si>
@@ -59,16 +71,22 @@
     <t xml:space="preserve">17.0%</t>
   </si>
   <si>
-    <t xml:space="preserve">Switzerland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.9%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.5%</t>
+    <t xml:space="preserve">49.3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43.7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54.8%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33.1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39.3%</t>
   </si>
   <si>
     <t xml:space="preserve">Spain</t>
@@ -83,22 +101,22 @@
     <t xml:space="preserve">59.0%</t>
   </si>
   <si>
-    <t xml:space="preserve">33.1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.6%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39.3%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49.3%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43.7%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54.8%</t>
+    <t xml:space="preserve">-1.8%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-7.3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.9%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.6%</t>
   </si>
   <si>
     <t xml:space="preserve">4.7%</t>
@@ -110,43 +128,25 @@
     <t xml:space="preserve">10.3%</t>
   </si>
   <si>
-    <t xml:space="preserve">3.9%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.6%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.8%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-7.3%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.1%</t>
+    <t xml:space="preserve">14.3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.9%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.2%</t>
   </si>
   <si>
     <t xml:space="preserve">16.8%</t>
   </si>
   <si>
     <t xml:space="preserve">21.5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.2%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14.3%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.7%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.9%</t>
   </si>
 </sst>
 </file>
@@ -521,22 +521,22 @@
         <v>11</v>
       </c>
       <c r="C2" t="n">
-        <v>4784981</v>
+        <v>2960800</v>
       </c>
       <c r="D2" t="n">
-        <v>81824</v>
+        <v>61805</v>
       </c>
       <c r="E2" t="n">
-        <v>73042</v>
+        <v>58355</v>
       </c>
       <c r="F2" t="n">
-        <v>8782</v>
+        <v>3451</v>
       </c>
       <c r="G2" t="n">
-        <v>4830</v>
+        <v>711</v>
       </c>
       <c r="H2" t="n">
-        <v>12435</v>
+        <v>6123</v>
       </c>
       <c r="I2" t="s">
         <v>12</v>
@@ -556,22 +556,22 @@
         <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>2960800</v>
+        <v>4784981</v>
       </c>
       <c r="D3" t="n">
-        <v>61805</v>
+        <v>81824</v>
       </c>
       <c r="E3" t="n">
-        <v>58355</v>
+        <v>73042</v>
       </c>
       <c r="F3" t="n">
-        <v>3451</v>
+        <v>8782</v>
       </c>
       <c r="G3" t="n">
-        <v>711</v>
+        <v>4830</v>
       </c>
       <c r="H3" t="n">
-        <v>6123</v>
+        <v>12435</v>
       </c>
       <c r="I3" t="s">
         <v>16</v>
@@ -588,34 +588,34 @@
         <v>1918</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3871870</v>
+      </c>
+      <c r="D4" t="n">
+        <v>75034</v>
+      </c>
+      <c r="E4" t="n">
+        <v>50256</v>
+      </c>
+      <c r="F4" t="n">
+        <v>24779</v>
+      </c>
+      <c r="G4" t="n">
+        <v>21958</v>
+      </c>
+      <c r="H4" t="n">
+        <v>27548</v>
+      </c>
+      <c r="I4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="n">
-        <v>21192701</v>
-      </c>
-      <c r="D4" t="n">
-        <v>695758</v>
-      </c>
-      <c r="E4" t="n">
-        <v>453698</v>
-      </c>
-      <c r="F4" t="n">
-        <v>242061</v>
-      </c>
-      <c r="G4" t="n">
-        <v>216201</v>
-      </c>
-      <c r="H4" t="n">
-        <v>267526</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>21</v>
-      </c>
-      <c r="K4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5">
@@ -623,7 +623,7 @@
         <v>1918</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C5" t="n">
         <v>5813850</v>
@@ -644,13 +644,13 @@
         <v>30895</v>
       </c>
       <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
         <v>23</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>24</v>
-      </c>
-      <c r="K5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -658,25 +658,25 @@
         <v>1918</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C6" t="n">
-        <v>3871870</v>
+        <v>21192701</v>
       </c>
       <c r="D6" t="n">
-        <v>75034</v>
+        <v>695758</v>
       </c>
       <c r="E6" t="n">
-        <v>50256</v>
+        <v>453698</v>
       </c>
       <c r="F6" t="n">
-        <v>24779</v>
+        <v>242061</v>
       </c>
       <c r="G6" t="n">
-        <v>21958</v>
+        <v>216201</v>
       </c>
       <c r="H6" t="n">
-        <v>27548</v>
+        <v>267526</v>
       </c>
       <c r="I6" t="s">
         <v>26</v>
@@ -693,25 +693,25 @@
         <v>1957</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C7" t="n">
-        <v>29499414</v>
+        <v>5130100</v>
       </c>
       <c r="D7" t="n">
-        <v>293502</v>
+        <v>51066</v>
       </c>
       <c r="E7" t="n">
-        <v>280210</v>
+        <v>52027</v>
       </c>
       <c r="F7" t="n">
-        <v>13292</v>
+        <v>-961</v>
       </c>
       <c r="G7" t="n">
-        <v>-3401</v>
+        <v>-3812</v>
       </c>
       <c r="H7" t="n">
-        <v>28970</v>
+        <v>1632</v>
       </c>
       <c r="I7" t="s">
         <v>29</v>
@@ -728,7 +728,7 @@
         <v>1957</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C8" t="n">
         <v>7388611</v>
@@ -763,25 +763,25 @@
         <v>1957</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C9" t="n">
-        <v>5130100</v>
+        <v>29499414</v>
       </c>
       <c r="D9" t="n">
-        <v>51066</v>
+        <v>293502</v>
       </c>
       <c r="E9" t="n">
-        <v>52027</v>
+        <v>280210</v>
       </c>
       <c r="F9" t="n">
-        <v>-961</v>
+        <v>13292</v>
       </c>
       <c r="G9" t="n">
-        <v>-3812</v>
+        <v>-3401</v>
       </c>
       <c r="H9" t="n">
-        <v>1632</v>
+        <v>28970</v>
       </c>
       <c r="I9" t="s">
         <v>35</v>
@@ -798,34 +798,34 @@
         <v>2020</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C10" t="n">
-        <v>47353706</v>
+        <v>8636560</v>
       </c>
       <c r="D10" t="n">
-        <v>492930</v>
+        <v>75570</v>
       </c>
       <c r="E10" t="n">
-        <v>422004</v>
+        <v>66093</v>
       </c>
       <c r="F10" t="n">
-        <v>70926</v>
+        <v>9478</v>
       </c>
       <c r="G10" t="n">
-        <v>50451</v>
+        <v>6380</v>
       </c>
       <c r="H10" t="n">
-        <v>90911</v>
+        <v>12482</v>
       </c>
       <c r="I10" t="s">
         <v>38</v>
       </c>
       <c r="J10" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="K10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -833,7 +833,7 @@
         <v>2020</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C11" t="n">
         <v>10379295</v>
@@ -854,13 +854,13 @@
         <v>11013</v>
       </c>
       <c r="I11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J11" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12">
@@ -868,31 +868,31 @@
         <v>2020</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C12" t="n">
-        <v>8636560</v>
+        <v>47353706</v>
       </c>
       <c r="D12" t="n">
-        <v>75570</v>
+        <v>492930</v>
       </c>
       <c r="E12" t="n">
-        <v>66093</v>
+        <v>422004</v>
       </c>
       <c r="F12" t="n">
-        <v>9478</v>
+        <v>70926</v>
       </c>
       <c r="G12" t="n">
-        <v>6380</v>
+        <v>50451</v>
       </c>
       <c r="H12" t="n">
-        <v>12482</v>
+        <v>90911</v>
       </c>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J12" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="K12" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
2021 update (4 CH & SE)
</commit_message>
<xml_diff>
--- a/paper/Table_1.xlsx
+++ b/paper/Table_1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -147,6 +147,21 @@
   </si>
   <si>
     <t xml:space="preserve">21.5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5.4%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.9%</t>
   </si>
 </sst>
 </file>
@@ -898,6 +913,95 @@
         <v>44</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="n">
+        <v>8636560</v>
+      </c>
+      <c r="D13" t="n">
+        <v>34454</v>
+      </c>
+      <c r="E13" t="n">
+        <v>34330</v>
+      </c>
+      <c r="F13" t="n">
+        <v>125</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-1850</v>
+      </c>
+      <c r="H13" t="n">
+        <v>2080</v>
+      </c>
+      <c r="I13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="n">
+        <v>10379295</v>
+      </c>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="n">
+        <v>47353706</v>
+      </c>
+      <c r="D15" t="n">
+        <v>234826</v>
+      </c>
+      <c r="E15" t="n">
+        <v>221664</v>
+      </c>
+      <c r="F15" t="n">
+        <v>13163</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-292</v>
+      </c>
+      <c r="H15" t="n">
+        <v>26482</v>
+      </c>
+      <c r="I15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
too many fig 2s ;) mod theme of model check gr
</commit_message>
<xml_diff>
--- a/paper/Table_1.xlsx
+++ b/paper/Table_1.xlsx
@@ -32,136 +32,136 @@
     <t xml:space="preserve">Excess</t>
   </si>
   <si>
-    <t xml:space="preserve">Excess_lci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Excess_uci</t>
+    <t xml:space="preserve">excess_cri</t>
   </si>
   <si>
     <t xml:space="preserve">Percent_excess</t>
   </si>
   <si>
-    <t xml:space="preserve">Percent_lci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent_uci</t>
+    <t xml:space="preserve">percent_cri</t>
   </si>
   <si>
     <t xml:space="preserve">Switzerland</t>
   </si>
   <si>
+    <t xml:space="preserve">(711, 6123)</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.9%</t>
   </si>
   <si>
-    <t xml:space="preserve">1.2%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.5%</t>
+    <t xml:space="preserve">(1.2%, 10.5%)</t>
   </si>
   <si>
     <t xml:space="preserve">Sweden</t>
   </si>
   <si>
+    <t xml:space="preserve">(4830, 12435)</t>
+  </si>
+  <si>
     <t xml:space="preserve">12.0%</t>
   </si>
   <si>
-    <t xml:space="preserve">6.6%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17.0%</t>
+    <t xml:space="preserve">(6.6%, 17.0%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21958, 27548)</t>
   </si>
   <si>
     <t xml:space="preserve">49.3%</t>
   </si>
   <si>
-    <t xml:space="preserve">43.7%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54.8%</t>
+    <t xml:space="preserve">(43.7%, 54.8%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20898, 30895)</t>
   </si>
   <si>
     <t xml:space="preserve">33.1%</t>
   </si>
   <si>
-    <t xml:space="preserve">26.6%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39.3%</t>
+    <t xml:space="preserve">(26.6%, 39.3%)</t>
   </si>
   <si>
     <t xml:space="preserve">Spain</t>
   </si>
   <si>
+    <t xml:space="preserve">(216201, 267526)</t>
+  </si>
+  <si>
     <t xml:space="preserve">53.4%</t>
   </si>
   <si>
-    <t xml:space="preserve">47.7%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59.0%</t>
+    <t xml:space="preserve">(47.7%, 59.0%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3812, 1632)</t>
   </si>
   <si>
     <t xml:space="preserve">-1.8%</t>
   </si>
   <si>
-    <t xml:space="preserve">-7.3%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.1%</t>
+    <t xml:space="preserve">(-7.3%, 3.1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(179, 5316)</t>
   </si>
   <si>
     <t xml:space="preserve">3.9%</t>
   </si>
   <si>
-    <t xml:space="preserve">0.3%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.6%</t>
+    <t xml:space="preserve">(0.3%, 7.6%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3401, 28970)</t>
   </si>
   <si>
     <t xml:space="preserve">4.7%</t>
   </si>
   <si>
-    <t xml:space="preserve">-1.2%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.3%</t>
+    <t xml:space="preserve">(-1.2%, 10.3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(6380, 12482)</t>
   </si>
   <si>
     <t xml:space="preserve">14.3%</t>
   </si>
   <si>
-    <t xml:space="preserve">9.7%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.9%</t>
+    <t xml:space="preserve">(9.7%, 18.9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4247, 11013)</t>
   </si>
   <si>
     <t xml:space="preserve">8.5%</t>
   </si>
   <si>
-    <t xml:space="preserve">12.2%</t>
+    <t xml:space="preserve">(4.7%, 12.2%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(50451, 90911)</t>
   </si>
   <si>
     <t xml:space="preserve">16.8%</t>
   </si>
   <si>
-    <t xml:space="preserve">21.5%</t>
+    <t xml:space="preserve">(12.0%, 21.5%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1850, 2080)</t>
   </si>
   <si>
     <t xml:space="preserve">0.4%</t>
   </si>
   <si>
-    <t xml:space="preserve">-5.4%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.9%</t>
+    <t xml:space="preserve">(-5.4%, 6.1%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-292, 26482)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-0.1%, 11.9%)</t>
   </si>
 </sst>
 </file>
@@ -521,19 +521,13 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1890</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" t="n">
         <v>2960800</v>
@@ -547,20 +541,14 @@
       <c r="F2" t="n">
         <v>3451</v>
       </c>
-      <c r="G2" t="n">
-        <v>711</v>
-      </c>
-      <c r="H2" t="n">
-        <v>6123</v>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
       </c>
       <c r="I2" t="s">
         <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -568,7 +556,7 @@
         <v>1890</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="n">
         <v>4784981</v>
@@ -582,20 +570,14 @@
       <c r="F3" t="n">
         <v>8782</v>
       </c>
-      <c r="G3" t="n">
-        <v>4830</v>
-      </c>
-      <c r="H3" t="n">
-        <v>12435</v>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
       </c>
       <c r="I3" t="s">
         <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -603,7 +585,7 @@
         <v>1918</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="n">
         <v>3871870</v>
@@ -617,20 +599,14 @@
       <c r="F4" t="n">
         <v>24779</v>
       </c>
-      <c r="G4" t="n">
-        <v>21958</v>
-      </c>
-      <c r="H4" t="n">
-        <v>27548</v>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
       </c>
       <c r="I4" t="s">
         <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5">
@@ -638,7 +614,7 @@
         <v>1918</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" t="n">
         <v>5813850</v>
@@ -652,20 +628,14 @@
       <c r="F5" t="n">
         <v>26022</v>
       </c>
-      <c r="G5" t="n">
-        <v>20898</v>
-      </c>
-      <c r="H5" t="n">
-        <v>30895</v>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
       </c>
       <c r="I5" t="s">
         <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6">
@@ -673,7 +643,7 @@
         <v>1918</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" t="n">
         <v>21192701</v>
@@ -687,20 +657,14 @@
       <c r="F6" t="n">
         <v>242061</v>
       </c>
-      <c r="G6" t="n">
-        <v>216201</v>
-      </c>
-      <c r="H6" t="n">
-        <v>267526</v>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
       </c>
       <c r="I6" t="s">
         <v>26</v>
-      </c>
-      <c r="J6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -708,7 +672,7 @@
         <v>1957</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="n">
         <v>5130100</v>
@@ -722,20 +686,14 @@
       <c r="F7" t="n">
         <v>-961</v>
       </c>
-      <c r="G7" t="n">
-        <v>-3812</v>
-      </c>
-      <c r="H7" t="n">
-        <v>1632</v>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
       </c>
       <c r="I7" t="s">
         <v>29</v>
-      </c>
-      <c r="J7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8">
@@ -743,7 +701,7 @@
         <v>1957</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" t="n">
         <v>7388611</v>
@@ -757,20 +715,14 @@
       <c r="F8" t="n">
         <v>2775</v>
       </c>
-      <c r="G8" t="n">
-        <v>179</v>
-      </c>
-      <c r="H8" t="n">
-        <v>5316</v>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
+        <v>31</v>
       </c>
       <c r="I8" t="s">
         <v>32</v>
-      </c>
-      <c r="J8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9">
@@ -778,7 +730,7 @@
         <v>1957</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" t="n">
         <v>29499414</v>
@@ -792,20 +744,14 @@
       <c r="F9" t="n">
         <v>13292</v>
       </c>
-      <c r="G9" t="n">
-        <v>-3401</v>
-      </c>
-      <c r="H9" t="n">
-        <v>28970</v>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>34</v>
       </c>
       <c r="I9" t="s">
         <v>35</v>
-      </c>
-      <c r="J9" t="s">
-        <v>36</v>
-      </c>
-      <c r="K9" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="10">
@@ -813,7 +759,7 @@
         <v>2020</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" t="n">
         <v>8636560</v>
@@ -827,20 +773,14 @@
       <c r="F10" t="n">
         <v>9478</v>
       </c>
-      <c r="G10" t="n">
-        <v>6380</v>
-      </c>
-      <c r="H10" t="n">
-        <v>12482</v>
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" t="s">
+        <v>37</v>
       </c>
       <c r="I10" t="s">
         <v>38</v>
-      </c>
-      <c r="J10" t="s">
-        <v>39</v>
-      </c>
-      <c r="K10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -848,7 +788,7 @@
         <v>2020</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" t="n">
         <v>10379295</v>
@@ -862,20 +802,14 @@
       <c r="F11" t="n">
         <v>7671</v>
       </c>
-      <c r="G11" t="n">
-        <v>4247</v>
-      </c>
-      <c r="H11" t="n">
-        <v>11013</v>
+      <c r="G11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" t="s">
+        <v>40</v>
       </c>
       <c r="I11" t="s">
         <v>41</v>
-      </c>
-      <c r="J11" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="12">
@@ -883,7 +817,7 @@
         <v>2020</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" t="n">
         <v>47353706</v>
@@ -897,19 +831,13 @@
       <c r="F12" t="n">
         <v>70926</v>
       </c>
-      <c r="G12" t="n">
-        <v>50451</v>
-      </c>
-      <c r="H12" t="n">
-        <v>90911</v>
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" t="s">
+        <v>43</v>
       </c>
       <c r="I12" t="s">
-        <v>43</v>
-      </c>
-      <c r="J12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" t="s">
         <v>44</v>
       </c>
     </row>
@@ -918,7 +846,7 @@
         <v>2021</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13" t="n">
         <v>8636560</v>
@@ -932,19 +860,13 @@
       <c r="F13" t="n">
         <v>125</v>
       </c>
-      <c r="G13" t="n">
-        <v>-1850</v>
-      </c>
-      <c r="H13" t="n">
-        <v>2080</v>
+      <c r="G13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" t="s">
+        <v>46</v>
       </c>
       <c r="I13" t="s">
-        <v>45</v>
-      </c>
-      <c r="J13" t="s">
-        <v>46</v>
-      </c>
-      <c r="K13" t="s">
         <v>47</v>
       </c>
     </row>
@@ -953,7 +875,7 @@
         <v>2021</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" t="n">
         <v>10379295</v>
@@ -964,15 +886,13 @@
       <c r="G14"/>
       <c r="H14"/>
       <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>2021</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" t="n">
         <v>47353706</v>
@@ -986,19 +906,13 @@
       <c r="F15" t="n">
         <v>13163</v>
       </c>
-      <c r="G15" t="n">
-        <v>-292</v>
-      </c>
-      <c r="H15" t="n">
-        <v>26482</v>
+      <c r="G15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
       </c>
       <c r="I15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" t="s">
-        <v>48</v>
-      </c>
-      <c r="K15" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new paths and new tables ready
</commit_message>
<xml_diff>
--- a/paper/Table_1.xlsx
+++ b/paper/Table_1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -29,9 +29,6 @@
     <t xml:space="preserve">Expected</t>
   </si>
   <si>
-    <t xml:space="preserve">Confirmed</t>
-  </si>
-  <si>
     <t xml:space="preserve">Deaths</t>
   </si>
   <si>
@@ -44,7 +41,7 @@
     <t xml:space="preserve">61,805</t>
   </si>
   <si>
-    <t xml:space="preserve">58,340</t>
+    <t xml:space="preserve">55,700-61,100</t>
   </si>
   <si>
     <t xml:space="preserve">--</t>
@@ -59,7 +56,7 @@
     <t xml:space="preserve">81,824</t>
   </si>
   <si>
-    <t xml:space="preserve">73,039</t>
+    <t xml:space="preserve">69,300-77,000</t>
   </si>
   <si>
     <t xml:space="preserve">3,878,360</t>
@@ -68,7 +65,7 @@
     <t xml:space="preserve">75,034</t>
   </si>
   <si>
-    <t xml:space="preserve">50,337</t>
+    <t xml:space="preserve">47,600-53,100</t>
   </si>
   <si>
     <t xml:space="preserve">5,802,022</t>
@@ -77,7 +74,7 @@
     <t xml:space="preserve">104,591</t>
   </si>
   <si>
-    <t xml:space="preserve">78,697</t>
+    <t xml:space="preserve">73,500-84,000</t>
   </si>
   <si>
     <t xml:space="preserve">Spain</t>
@@ -89,7 +86,7 @@
     <t xml:space="preserve">695,758</t>
   </si>
   <si>
-    <t xml:space="preserve">453,827</t>
+    <t xml:space="preserve">429,700-480,000</t>
   </si>
   <si>
     <t xml:space="preserve">5,097,745</t>
@@ -98,7 +95,7 @@
     <t xml:space="preserve">51,066</t>
   </si>
   <si>
-    <t xml:space="preserve">51,995</t>
+    <t xml:space="preserve">49,300-54,700</t>
   </si>
   <si>
     <t xml:space="preserve">7,341,017</t>
@@ -107,7 +104,7 @@
     <t xml:space="preserve">73,132</t>
   </si>
   <si>
-    <t xml:space="preserve">70,389</t>
+    <t xml:space="preserve">67,800-73,000</t>
   </si>
   <si>
     <t xml:space="preserve">29,445,865</t>
@@ -116,7 +113,7 @@
     <t xml:space="preserve">293,502</t>
   </si>
   <si>
-    <t xml:space="preserve">279,917</t>
+    <t xml:space="preserve">264,700-296,200</t>
   </si>
   <si>
     <t xml:space="preserve">8,605,965</t>
@@ -125,10 +122,7 @@
     <t xml:space="preserve">76,195</t>
   </si>
   <si>
-    <t xml:space="preserve">67,718</t>
-  </si>
-  <si>
-    <t xml:space="preserve">452,296</t>
+    <t xml:space="preserve">64,700-70,900</t>
   </si>
   <si>
     <t xml:space="preserve">7,873</t>
@@ -140,10 +134,7 @@
     <t xml:space="preserve">97,870</t>
   </si>
   <si>
-    <t xml:space="preserve">90,205</t>
-  </si>
-  <si>
-    <t xml:space="preserve">437,379</t>
+    <t xml:space="preserve">86,900-93,700</t>
   </si>
   <si>
     <t xml:space="preserve">8,727</t>
@@ -155,10 +146,7 @@
     <t xml:space="preserve">492,930</t>
   </si>
   <si>
-    <t xml:space="preserve">421,014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,928,265</t>
+    <t xml:space="preserve">400,500-441,000</t>
   </si>
   <si>
     <t xml:space="preserve">50,837</t>
@@ -170,10 +158,7 @@
     <t xml:space="preserve">34,619</t>
   </si>
   <si>
-    <t xml:space="preserve">35,618</t>
-  </si>
-  <si>
-    <t xml:space="preserve">250,880</t>
+    <t xml:space="preserve">33,700-37,700</t>
   </si>
   <si>
     <t xml:space="preserve">2,900</t>
@@ -182,9 +167,6 @@
     <t xml:space="preserve">10,379,295</t>
   </si>
   <si>
-    <t xml:space="preserve">653,174</t>
-  </si>
-  <si>
     <t xml:space="preserve">5,903</t>
   </si>
   <si>
@@ -194,10 +176,7 @@
     <t xml:space="preserve">234,994</t>
   </si>
   <si>
-    <t xml:space="preserve">224,044</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,893,040</t>
+    <t xml:space="preserve">210,600-238,500</t>
   </si>
   <si>
     <t xml:space="preserve">30,046</t>
@@ -551,31 +530,25 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1890</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
       <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -583,22 +556,19 @@
         <v>1890</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
       <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -606,22 +576,19 @@
         <v>1918</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
       <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -629,22 +596,19 @@
         <v>1918</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
       <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -652,22 +616,19 @@
         <v>1918</v>
       </c>
       <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
       <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -675,22 +636,19 @@
         <v>1957</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
       <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -698,22 +656,19 @@
         <v>1957</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
       <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -721,22 +676,19 @@
         <v>1957</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>33</v>
       </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
       <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -744,22 +696,19 @@
         <v>2020</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>36</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>37</v>
-      </c>
-      <c r="F10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11">
@@ -767,22 +716,19 @@
         <v>2020</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
         <v>40</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>41</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12">
@@ -790,22 +736,19 @@
         <v>2020</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
         <v>45</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13">
@@ -813,22 +756,19 @@
         <v>2021</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14">
@@ -836,18 +776,19 @@
         <v>2021</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14"/>
-      <c r="E14"/>
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
       <c r="F14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15">
@@ -855,22 +796,19 @@
         <v>2021</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adapted table 2, new proposition for figure 2
</commit_message>
<xml_diff>
--- a/paper/Table_1.xlsx
+++ b/paper/Table_1.xlsx
@@ -41,7 +41,7 @@
     <t xml:space="preserve">61,805</t>
   </si>
   <si>
-    <t xml:space="preserve">55,700-61,100</t>
+    <t xml:space="preserve">55,700 to 61,100</t>
   </si>
   <si>
     <t xml:space="preserve">--</t>
@@ -56,7 +56,7 @@
     <t xml:space="preserve">81,824</t>
   </si>
   <si>
-    <t xml:space="preserve">69,300-77,000</t>
+    <t xml:space="preserve">69,300 to 77,000</t>
   </si>
   <si>
     <t xml:space="preserve">3,878,360</t>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">75,034</t>
   </si>
   <si>
-    <t xml:space="preserve">47,600-53,100</t>
+    <t xml:space="preserve">47,600 to 53,100</t>
   </si>
   <si>
     <t xml:space="preserve">5,802,022</t>
@@ -74,7 +74,7 @@
     <t xml:space="preserve">104,591</t>
   </si>
   <si>
-    <t xml:space="preserve">73,500-84,000</t>
+    <t xml:space="preserve">73,500 to 84,000</t>
   </si>
   <si>
     <t xml:space="preserve">Spain</t>
@@ -86,7 +86,7 @@
     <t xml:space="preserve">695,758</t>
   </si>
   <si>
-    <t xml:space="preserve">429,700-480,000</t>
+    <t xml:space="preserve">429,700 to 480,000</t>
   </si>
   <si>
     <t xml:space="preserve">5,097,745</t>
@@ -95,7 +95,7 @@
     <t xml:space="preserve">51,066</t>
   </si>
   <si>
-    <t xml:space="preserve">49,300-54,700</t>
+    <t xml:space="preserve">49,300 to 54,700</t>
   </si>
   <si>
     <t xml:space="preserve">7,341,017</t>
@@ -104,7 +104,7 @@
     <t xml:space="preserve">73,132</t>
   </si>
   <si>
-    <t xml:space="preserve">67,800-73,000</t>
+    <t xml:space="preserve">67,800 to 73,000</t>
   </si>
   <si>
     <t xml:space="preserve">29,445,865</t>
@@ -113,7 +113,7 @@
     <t xml:space="preserve">293,502</t>
   </si>
   <si>
-    <t xml:space="preserve">264,700-296,200</t>
+    <t xml:space="preserve">264,700 to 296,200</t>
   </si>
   <si>
     <t xml:space="preserve">8,605,965</t>
@@ -122,7 +122,7 @@
     <t xml:space="preserve">76,195</t>
   </si>
   <si>
-    <t xml:space="preserve">64,700-70,900</t>
+    <t xml:space="preserve">64,700 to 70,900</t>
   </si>
   <si>
     <t xml:space="preserve">7,873</t>
@@ -134,7 +134,7 @@
     <t xml:space="preserve">97,870</t>
   </si>
   <si>
-    <t xml:space="preserve">86,900-93,700</t>
+    <t xml:space="preserve">86,900 to 93,700</t>
   </si>
   <si>
     <t xml:space="preserve">8,727</t>
@@ -146,7 +146,7 @@
     <t xml:space="preserve">492,930</t>
   </si>
   <si>
-    <t xml:space="preserve">400,500-441,000</t>
+    <t xml:space="preserve">400,500 to 441,000</t>
   </si>
   <si>
     <t xml:space="preserve">50,837</t>
@@ -158,7 +158,7 @@
     <t xml:space="preserve">34,619</t>
   </si>
   <si>
-    <t xml:space="preserve">33,700-37,700</t>
+    <t xml:space="preserve">33,700 to 37,700</t>
   </si>
   <si>
     <t xml:space="preserve">2,900</t>
@@ -176,7 +176,7 @@
     <t xml:space="preserve">234,994</t>
   </si>
   <si>
-    <t xml:space="preserve">210,300-238,400</t>
+    <t xml:space="preserve">210,300 to 238,400</t>
   </si>
   <si>
     <t xml:space="preserve">30,046</t>

</xml_diff>

<commit_message>
table1 with journal's edits
</commit_message>
<xml_diff>
--- a/paper/Table_1.xlsx
+++ b/paper/Table_1.xlsx
@@ -35,13 +35,13 @@
     <t xml:space="preserve">Switzerland</t>
   </si>
   <si>
-    <t xml:space="preserve">2,949,868</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61,805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55,700 to 61,100</t>
+    <t xml:space="preserve">2 949 868</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61 805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55 700 to 61 100</t>
   </si>
   <si>
     <t xml:space="preserve">--</t>
@@ -50,136 +50,136 @@
     <t xml:space="preserve">Sweden</t>
   </si>
   <si>
-    <t xml:space="preserve">4,775,819</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81,824</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69,300 to 77,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,878,360</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75,034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47,600 to 53,100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,802,022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">104,591</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73,500 to 84,000</t>
+    <t xml:space="preserve">4 775 819</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81 824</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69 300 to 77 000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 878 360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75 034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47 600 to 53 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 802 022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">104 591</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73 500 to 84 000</t>
   </si>
   <si>
     <t xml:space="preserve">Spain</t>
   </si>
   <si>
-    <t xml:space="preserve">21,300,235</t>
-  </si>
-  <si>
-    <t xml:space="preserve">695,758</t>
-  </si>
-  <si>
-    <t xml:space="preserve">429,700 to 480,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,097,745</t>
-  </si>
-  <si>
-    <t xml:space="preserve">51,066</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49,300 to 54,700</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,341,017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73,132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67,800 to 73,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29,445,865</t>
-  </si>
-  <si>
-    <t xml:space="preserve">293,502</t>
-  </si>
-  <si>
-    <t xml:space="preserve">264,700 to 296,200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,605,965</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76,195</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64,700 to 70,900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,873</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,327,496</t>
-  </si>
-  <si>
-    <t xml:space="preserve">97,870</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86,900 to 93,700</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,727</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47,332,613</t>
-  </si>
-  <si>
-    <t xml:space="preserve">492,930</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400,500 to 441,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50,837</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,670,302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34,619</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33,700 to 37,700</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,379,295</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,903</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47,394,223</t>
-  </si>
-  <si>
-    <t xml:space="preserve">234,994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">210,300 to 238,400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30,046</t>
+    <t xml:space="preserve">21 300 235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">695 758</t>
+  </si>
+  <si>
+    <t xml:space="preserve">429 700 to 480 000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 097 745</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51 066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49 300 to 54 700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 341 017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73 132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67 800 to 73 000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 445 865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">293 502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">264 700 to 296 200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 605 965</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76 195</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64 700 to 70 900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 873</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 327 496</t>
+  </si>
+  <si>
+    <t xml:space="preserve">97 870</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86 900 to 93 700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 727</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47 332 613</t>
+  </si>
+  <si>
+    <t xml:space="preserve">492 930</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400 500 to 441 000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 837</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 670 302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34 619</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33 700 to 37 700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 379 295</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 903</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47 394 223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">234 994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">210 300 to 238 400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 046</t>
   </si>
 </sst>
 </file>

</xml_diff>